<commit_message>
Fixed Multi-scaling model #3
</commit_message>
<xml_diff>
--- a/Confusion matrix/ms3_confusion_matrix.xlsx
+++ b/Confusion matrix/ms3_confusion_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jasmine Moreno\Documents\GitHub\ee211\Confusion matrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E566A0E7-9058-404F-89FF-4A1DFF36DBA6}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC77C89-40AE-4E61-AE60-AB68AEFF3090}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17268" windowHeight="5436" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -121,16 +121,16 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -171,22 +171,22 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -493,109 +493,90 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P12" workbookViewId="0">
-      <selection activeCell="AD22" sqref="AD22"/>
+    <sheetView tabSelected="1" topLeftCell="W7" workbookViewId="0">
+      <selection activeCell="AE14" sqref="AE14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="2.47265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="1.83984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="1.7890625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="1.734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="1.89453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="1.68359375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="1.9453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="1.89453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="1.68359375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="1.734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="1.68359375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="2.3671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="1.9453125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="1.734375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="3.68359375" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="1.68359375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="1.9453125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="1.83984375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="2.47265625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="1.734375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="1.68359375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.47265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="17" width="3.68359375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="2.68359375" bestFit="1" customWidth="1"/>
+    <col min="19" max="25" width="3.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="2"/>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="3" t="s">
         <v>23</v>
       </c>
       <c r="Z1" s="4"/>
@@ -612,11 +593,11 @@
       <c r="AG1" s="5"/>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>331</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -664,7 +645,7 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>331</v>
+        <v>0</v>
       </c>
       <c r="S2">
         <v>0</v>
@@ -691,29 +672,33 @@
         <v>0</v>
       </c>
       <c r="AB2">
-        <f xml:space="preserve"> B2/SUM(B2:B25,0.0001)</f>
-        <v>0</v>
+        <f xml:space="preserve"> B2/SUM(B2:B25)</f>
+        <v>0.85309278350515461</v>
       </c>
       <c r="AC2">
         <f>B2/SUM(B2:Y2)</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="AE2">
+        <f>SUM(C3,B2,D4,E5,F6,G7,H8,I9,J10,K11,L12,M13,N14,O15,P16,Q17,R18,S19,T20,U21,V22,W23,X24,Y25)/SUM(B2:Y25)</f>
+        <v>0.78750697155605132</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>410</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -731,7 +716,7 @@
         <v>0</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -752,7 +737,7 @@
         <v>0</v>
       </c>
       <c r="R3">
-        <v>432</v>
+        <v>0</v>
       </c>
       <c r="S3">
         <v>0</v>
@@ -779,16 +764,16 @@
         <v>1</v>
       </c>
       <c r="AB3">
-        <f>C3/SUM(C2:C25,0.0001)</f>
-        <v>0</v>
+        <f>C3/SUM(C2:C25)</f>
+        <v>1</v>
       </c>
       <c r="AC3">
         <f>C3/SUM(B3:Y3)</f>
-        <v>0</v>
+        <v>0.94907407407407407</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4">
@@ -798,7 +783,7 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>307</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -822,7 +807,7 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -840,7 +825,7 @@
         <v>0</v>
       </c>
       <c r="R4">
-        <v>310</v>
+        <v>0</v>
       </c>
       <c r="S4">
         <v>0</v>
@@ -867,16 +852,16 @@
         <v>2</v>
       </c>
       <c r="AB4">
-        <f xml:space="preserve"> D4/SUM(D2:D25,0.0001)</f>
-        <v>0</v>
+        <f xml:space="preserve"> D4/SUM(D2:D25)</f>
+        <v>0.91641791044776122</v>
       </c>
       <c r="AC4">
         <f>D4/SUM(B4:Y4)</f>
-        <v>0</v>
+        <v>0.99032258064516132</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5">
@@ -889,7 +874,7 @@
         <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>222</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -916,7 +901,7 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O5">
         <v>0</v>
@@ -928,7 +913,7 @@
         <v>0</v>
       </c>
       <c r="R5">
-        <v>245</v>
+        <v>0</v>
       </c>
       <c r="S5">
         <v>0</v>
@@ -946,7 +931,7 @@
         <v>0</v>
       </c>
       <c r="X5">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="Y5">
         <v>0</v>
@@ -955,15 +940,16 @@
         <v>3</v>
       </c>
       <c r="AB5">
-        <v>0</v>
+        <f>E5/SUM(E2:E25)</f>
+        <v>0.92116182572614103</v>
       </c>
       <c r="AC5">
         <f>E5/SUM(B5:Y5)</f>
-        <v>0</v>
+        <v>0.90612244897959182</v>
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B6">
@@ -979,7 +965,7 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>455</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -1015,10 +1001,10 @@
         <v>0</v>
       </c>
       <c r="R6">
-        <v>498</v>
+        <v>0</v>
       </c>
       <c r="S6">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="T6">
         <v>0</v>
@@ -1042,15 +1028,16 @@
         <v>4</v>
       </c>
       <c r="AB6">
-        <v>0</v>
+        <f xml:space="preserve"> F6/SUM(F2:F25)</f>
+        <v>0.86832061068702293</v>
       </c>
       <c r="AC6">
         <f>F6/SUM(B6:Y6)</f>
-        <v>0</v>
+        <v>0.91365461847389562</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7">
@@ -1060,7 +1047,7 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -1069,7 +1056,7 @@
         <v>0</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>220</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -1102,7 +1089,7 @@
         <v>0</v>
       </c>
       <c r="R7">
-        <v>247</v>
+        <v>0</v>
       </c>
       <c r="S7">
         <v>0</v>
@@ -1114,7 +1101,7 @@
         <v>0</v>
       </c>
       <c r="V7">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="W7">
         <v>0</v>
@@ -1129,15 +1116,16 @@
         <v>5</v>
       </c>
       <c r="AB7">
-        <v>0</v>
+        <f>G7/SUM(G2:G25)</f>
+        <v>0.84615384615384615</v>
       </c>
       <c r="AC7">
         <f>G7/SUM(B7:Y7)</f>
-        <v>0</v>
+        <v>0.89068825910931171</v>
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8">
@@ -1159,10 +1147,10 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>258</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -1177,25 +1165,25 @@
         <v>0</v>
       </c>
       <c r="N8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="O8">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P8">
         <v>0</v>
       </c>
       <c r="Q8">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="R8">
-        <v>348</v>
+        <v>0</v>
       </c>
       <c r="S8">
         <v>0</v>
       </c>
       <c r="T8">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="U8">
         <v>0</v>
@@ -1216,15 +1204,16 @@
         <v>6</v>
       </c>
       <c r="AB8">
-        <v>0</v>
+        <f xml:space="preserve"> H8/SUM(H2:H25)</f>
+        <v>0.8716216216216216</v>
       </c>
       <c r="AC8">
         <f>H8/SUM(B8:Y8)</f>
-        <v>0</v>
+        <v>0.74137931034482762</v>
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9">
@@ -1246,10 +1235,10 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>390</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -1276,13 +1265,13 @@
         <v>0</v>
       </c>
       <c r="R9">
-        <v>436</v>
+        <v>0</v>
       </c>
       <c r="S9">
         <v>0</v>
       </c>
       <c r="T9">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="U9">
         <v>0</v>
@@ -1303,19 +1292,20 @@
         <v>7</v>
       </c>
       <c r="AB9">
-        <v>0</v>
+        <f>I9/SUM(I2:I25)</f>
+        <v>0.98734177215189878</v>
       </c>
       <c r="AC9">
         <f>I9/SUM(B9:Y9)</f>
-        <v>0</v>
+        <v>0.89449541284403666</v>
       </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1324,7 +1314,7 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -1339,19 +1329,19 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>243</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M10">
         <v>0</v>
       </c>
       <c r="N10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O10">
         <v>0</v>
@@ -1363,13 +1353,13 @@
         <v>0</v>
       </c>
       <c r="R10">
-        <v>288</v>
+        <v>0</v>
       </c>
       <c r="S10">
         <v>0</v>
       </c>
       <c r="T10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U10">
         <v>0</v>
@@ -1378,27 +1368,28 @@
         <v>0</v>
       </c>
       <c r="W10">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="X10">
         <v>0</v>
       </c>
       <c r="Y10">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AA10" s="6" t="s">
         <v>8</v>
       </c>
       <c r="AB10">
-        <v>0</v>
+        <f>J10/SUM(J2:J25)</f>
+        <v>0.75937500000000002</v>
       </c>
       <c r="AC10">
         <f xml:space="preserve"> J10/SUM(B10:Y10)</f>
-        <v>0</v>
+        <v>0.84375</v>
       </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B11">
@@ -1417,7 +1408,7 @@
         <v>0</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1426,10 +1417,10 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>221</v>
       </c>
       <c r="L11">
         <v>0</v>
@@ -1450,7 +1441,7 @@
         <v>0</v>
       </c>
       <c r="R11">
-        <v>331</v>
+        <v>44</v>
       </c>
       <c r="S11">
         <v>0</v>
@@ -1459,10 +1450,10 @@
         <v>0</v>
       </c>
       <c r="U11">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="V11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W11">
         <v>0</v>
@@ -1471,21 +1462,22 @@
         <v>0</v>
       </c>
       <c r="Y11">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AA11" s="6" t="s">
         <v>9</v>
       </c>
       <c r="AB11">
-        <v>0</v>
+        <f>K11/SUM(K2:K25)</f>
+        <v>0.66566265060240959</v>
       </c>
       <c r="AC11">
         <f>K11/SUM(B11:Y11)</f>
-        <v>0</v>
+        <v>0.66767371601208458</v>
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B12">
@@ -1519,7 +1511,7 @@
         <v>0</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>209</v>
       </c>
       <c r="M12">
         <v>0</v>
@@ -1537,7 +1529,7 @@
         <v>0</v>
       </c>
       <c r="R12">
-        <v>209</v>
+        <v>0</v>
       </c>
       <c r="S12">
         <v>0</v>
@@ -1564,15 +1556,16 @@
         <v>10</v>
       </c>
       <c r="AB12">
-        <v>0</v>
+        <f>L12/SUM(L2:L25)</f>
+        <v>0.8132295719844358</v>
       </c>
       <c r="AC12">
         <f xml:space="preserve"> L12/SUM(B12:Y12)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B13">
@@ -1588,7 +1581,7 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="G13">
         <v>0</v>
@@ -1609,10 +1602,10 @@
         <v>0</v>
       </c>
       <c r="M13">
-        <v>0</v>
+        <v>301</v>
       </c>
       <c r="N13">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="O13">
         <v>0</v>
@@ -1624,10 +1617,10 @@
         <v>0</v>
       </c>
       <c r="R13">
-        <v>394</v>
+        <v>0</v>
       </c>
       <c r="S13">
-        <v>0</v>
+        <v>51</v>
       </c>
       <c r="T13">
         <v>0</v>
@@ -1651,19 +1644,20 @@
         <v>11</v>
       </c>
       <c r="AB13">
-        <v>0</v>
+        <f xml:space="preserve"> M13/SUM(M2:M25)</f>
+        <v>0.78590078328981727</v>
       </c>
       <c r="AC13">
         <f>M13/SUM(B13:Y13)</f>
-        <v>0</v>
+        <v>0.76395939086294418</v>
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="C14">
         <v>0</v>
@@ -1672,7 +1666,7 @@
         <v>0</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -1696,10 +1690,10 @@
         <v>0</v>
       </c>
       <c r="M14">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="N14">
-        <v>0</v>
+        <v>187</v>
       </c>
       <c r="O14">
         <v>0</v>
@@ -1708,16 +1702,16 @@
         <v>0</v>
       </c>
       <c r="Q14">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="R14">
-        <v>291</v>
+        <v>0</v>
       </c>
       <c r="S14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T14">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="U14">
         <v>0</v>
@@ -1738,15 +1732,16 @@
         <v>12</v>
       </c>
       <c r="AB14">
-        <v>0</v>
+        <f>N14/SUM(N2:N25)</f>
+        <v>0.80257510729613735</v>
       </c>
       <c r="AC14">
         <f xml:space="preserve"> N14/SUM(B14:Y14)</f>
-        <v>0</v>
+        <v>0.6426116838487973</v>
       </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15">
@@ -1756,19 +1751,19 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I15">
         <v>0</v>
@@ -1789,22 +1784,22 @@
         <v>0</v>
       </c>
       <c r="O15">
-        <v>0</v>
+        <v>183</v>
       </c>
       <c r="P15">
         <v>0</v>
       </c>
       <c r="Q15">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="R15">
-        <v>246</v>
+        <v>0</v>
       </c>
       <c r="S15">
         <v>0</v>
       </c>
       <c r="T15">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="U15">
         <v>0</v>
@@ -1825,15 +1820,16 @@
         <v>13</v>
       </c>
       <c r="AB15">
-        <v>0</v>
+        <f>O15/SUM(O2:O25)</f>
+        <v>0.98918918918918919</v>
       </c>
       <c r="AC15">
         <f>O15/SUM(B15:Y15)</f>
-        <v>0</v>
+        <v>0.74390243902439024</v>
       </c>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B16">
@@ -1879,13 +1875,13 @@
         <v>0</v>
       </c>
       <c r="P16">
-        <v>0</v>
+        <v>347</v>
       </c>
       <c r="Q16">
         <v>0</v>
       </c>
       <c r="R16">
-        <v>347</v>
+        <v>0</v>
       </c>
       <c r="S16">
         <v>0</v>
@@ -1912,19 +1908,20 @@
         <v>14</v>
       </c>
       <c r="AB16">
-        <v>0</v>
+        <f>P16/SUM(P2:P25)</f>
+        <v>1</v>
       </c>
       <c r="AC16">
         <f>P16/SUM(B16:Y16)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C17">
         <v>0</v>
@@ -1957,7 +1954,7 @@
         <v>0</v>
       </c>
       <c r="M17">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="N17">
         <v>0</v>
@@ -1969,10 +1966,10 @@
         <v>0</v>
       </c>
       <c r="Q17">
-        <v>0</v>
+        <v>143</v>
       </c>
       <c r="R17">
-        <v>164</v>
+        <v>0</v>
       </c>
       <c r="S17">
         <v>0</v>
@@ -1999,15 +1996,16 @@
         <v>15</v>
       </c>
       <c r="AB17">
-        <v>0</v>
+        <f>Q17/SUM(Q2:Q25)</f>
+        <v>0.71144278606965172</v>
       </c>
       <c r="AC17">
         <f>Q17/SUM(B17:Y17)</f>
-        <v>0</v>
+        <v>0.87195121951219512</v>
       </c>
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B18">
@@ -2038,10 +2036,10 @@
         <v>0</v>
       </c>
       <c r="K18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L18">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="M18">
         <v>0</v>
@@ -2059,16 +2057,16 @@
         <v>0</v>
       </c>
       <c r="R18">
-        <v>144</v>
+        <v>72</v>
       </c>
       <c r="S18">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="T18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U18">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="V18">
         <v>0</v>
@@ -2087,15 +2085,15 @@
       </c>
       <c r="AB18">
         <f>R18/SUM(R2:R25)</f>
-        <v>2.0078081427774678E-2</v>
+        <v>0.36363636363636365</v>
       </c>
       <c r="AC18">
         <f xml:space="preserve"> R18/SUM(B18:Y18)</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B19">
@@ -2111,7 +2109,7 @@
         <v>0</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="G19">
         <v>0</v>
@@ -2123,7 +2121,7 @@
         <v>0</v>
       </c>
       <c r="J19">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="K19">
         <v>0</v>
@@ -2132,10 +2130,10 @@
         <v>0</v>
       </c>
       <c r="M19">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="N19">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O19">
         <v>0</v>
@@ -2147,10 +2145,10 @@
         <v>0</v>
       </c>
       <c r="R19">
-        <v>246</v>
+        <v>0</v>
       </c>
       <c r="S19">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="T19">
         <v>0</v>
@@ -2174,15 +2172,16 @@
         <v>17</v>
       </c>
       <c r="AB19">
-        <v>0</v>
+        <f>S19/SUM(S2:S25)</f>
+        <v>0.45112781954887216</v>
       </c>
       <c r="AC19">
         <f>S19/SUM(B19:Y19)</f>
-        <v>0</v>
+        <v>0.48780487804878048</v>
       </c>
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B20">
@@ -2216,7 +2215,7 @@
         <v>0</v>
       </c>
       <c r="L20">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="M20">
         <v>0</v>
@@ -2234,13 +2233,13 @@
         <v>0</v>
       </c>
       <c r="R20">
-        <v>248</v>
+        <v>0</v>
       </c>
       <c r="S20">
         <v>0</v>
       </c>
       <c r="T20">
-        <v>0</v>
+        <v>183</v>
       </c>
       <c r="U20">
         <v>0</v>
@@ -2252,7 +2251,7 @@
         <v>0</v>
       </c>
       <c r="X20">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="Y20">
         <v>0</v>
@@ -2261,15 +2260,16 @@
         <v>18</v>
       </c>
       <c r="AB20">
-        <v>0</v>
+        <f>T20/SUM(T2:T25)</f>
+        <v>0.52285714285714291</v>
       </c>
       <c r="AC20">
         <f>T20/SUM(B20:Y20)</f>
-        <v>0</v>
+        <v>0.73790322580645162</v>
       </c>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B21">
@@ -2282,7 +2282,7 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -2300,7 +2300,7 @@
         <v>0</v>
       </c>
       <c r="K21">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="L21">
         <v>0</v>
@@ -2321,7 +2321,7 @@
         <v>0</v>
       </c>
       <c r="R21">
-        <v>266</v>
+        <v>25</v>
       </c>
       <c r="S21">
         <v>0</v>
@@ -2330,10 +2330,10 @@
         <v>0</v>
       </c>
       <c r="U21">
-        <v>0</v>
+        <v>141</v>
       </c>
       <c r="V21">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="W21">
         <v>0</v>
@@ -2342,21 +2342,22 @@
         <v>0</v>
       </c>
       <c r="Y21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA21" s="6" t="s">
         <v>19</v>
       </c>
       <c r="AB21">
-        <v>0</v>
+        <f>U21/SUM(U2:U25)</f>
+        <v>0.6</v>
       </c>
       <c r="AC21">
         <f>U21/SUM(B21:Y21)</f>
-        <v>0</v>
+        <v>0.53007518796992481</v>
       </c>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B22">
@@ -2375,7 +2376,7 @@
         <v>0</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="H22">
         <v>0</v>
@@ -2384,10 +2385,10 @@
         <v>0</v>
       </c>
       <c r="J22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K22">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L22">
         <v>0</v>
@@ -2408,25 +2409,25 @@
         <v>0</v>
       </c>
       <c r="R22">
-        <v>346</v>
+        <v>29</v>
       </c>
       <c r="S22">
         <v>0</v>
       </c>
       <c r="T22">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="U22">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="V22">
-        <v>0</v>
+        <v>185</v>
       </c>
       <c r="W22">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="X22">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="Y22">
         <v>0</v>
@@ -2435,15 +2436,16 @@
         <v>20</v>
       </c>
       <c r="AB22">
-        <v>0</v>
+        <f>V22/SUM(V2:V25)</f>
+        <v>0.7007575757575758</v>
       </c>
       <c r="AC22">
         <f xml:space="preserve"> V22/SUM(B22:Y22)</f>
-        <v>0</v>
+        <v>0.53468208092485547</v>
       </c>
     </row>
     <row r="23" spans="1:29" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B23">
@@ -2495,7 +2497,7 @@
         <v>0</v>
       </c>
       <c r="R23">
-        <v>206</v>
+        <v>7</v>
       </c>
       <c r="S23">
         <v>0</v>
@@ -2504,13 +2506,13 @@
         <v>0</v>
       </c>
       <c r="U23">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="V23">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="W23">
-        <v>0</v>
+        <v>137</v>
       </c>
       <c r="X23">
         <v>0</v>
@@ -2522,15 +2524,16 @@
         <v>21</v>
       </c>
       <c r="AB23">
-        <v>0</v>
+        <f>W23/SUM(W2:W25)</f>
+        <v>0.53307392996108949</v>
       </c>
       <c r="AC23">
         <f>W23/SUM(B23:Y23)</f>
-        <v>0</v>
+        <v>0.66504854368932043</v>
       </c>
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B24">
@@ -2564,7 +2567,7 @@
         <v>0</v>
       </c>
       <c r="L24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M24">
         <v>0</v>
@@ -2582,13 +2585,13 @@
         <v>0</v>
       </c>
       <c r="R24">
-        <v>267</v>
+        <v>1</v>
       </c>
       <c r="S24">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="T24">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="U24">
         <v>0</v>
@@ -2597,10 +2600,10 @@
         <v>0</v>
       </c>
       <c r="W24">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="X24">
-        <v>0</v>
+        <v>182</v>
       </c>
       <c r="Y24">
         <v>0</v>
@@ -2609,15 +2612,16 @@
         <v>22</v>
       </c>
       <c r="AB24">
-        <v>0</v>
+        <f>X24/SUM(X2:X25)</f>
+        <v>0.69465648854961837</v>
       </c>
       <c r="AC24">
         <f>X24/SUM(B24:Y24)</f>
-        <v>0</v>
+        <v>0.68164794007490637</v>
       </c>
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B25">
@@ -2630,7 +2634,7 @@
         <v>0</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -2645,10 +2649,10 @@
         <v>0</v>
       </c>
       <c r="J25">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="K25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L25">
         <v>0</v>
@@ -2669,19 +2673,19 @@
         <v>0</v>
       </c>
       <c r="R25">
-        <v>332</v>
+        <v>20</v>
       </c>
       <c r="S25">
         <v>0</v>
       </c>
       <c r="T25">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="U25">
         <v>0</v>
       </c>
       <c r="V25">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="W25">
         <v>0</v>
@@ -2690,17 +2694,18 @@
         <v>0</v>
       </c>
       <c r="Y25">
-        <v>0</v>
+        <v>201</v>
       </c>
       <c r="AA25" s="6" t="s">
         <v>23</v>
       </c>
       <c r="AB25">
-        <v>0</v>
+        <f>Y25/SUM(Y2:Y25)</f>
+        <v>0.86266094420600858</v>
       </c>
       <c r="AC25">
         <f>Y25/SUM(B25:Y25)</f>
-        <v>0</v>
+        <v>0.60542168674698793</v>
       </c>
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.55000000000000004">
@@ -2709,11 +2714,11 @@
       </c>
       <c r="AB27">
         <f>AVERAGE(AB2:AB25)</f>
-        <v>8.3658672615727825E-4</v>
+        <v>0.77167732180173998</v>
       </c>
       <c r="AC27">
         <f>AVERAGE(AC2:AC25)</f>
-        <v>4.1666666666666664E-2</v>
+        <v>0.77342369570802239</v>
       </c>
     </row>
   </sheetData>

</xml_diff>